<commit_message>
The images were updated according to the changes in DB
</commit_message>
<xml_diff>
--- a/images/statistics_table.xlsx
+++ b/images/statistics_table.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Archaea</t>
   </si>
@@ -90,6 +90,27 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>kingdom</t>
+  </si>
+  <si>
+    <t>phylum2</t>
+  </si>
+  <si>
+    <t>total_orgs</t>
+  </si>
+  <si>
+    <t>orgs_with_M</t>
+  </si>
+  <si>
+    <t>num_M_genes</t>
+  </si>
+  <si>
+    <t>orgs_with_bchlD_fs</t>
+  </si>
+  <si>
+    <t>num_bchlD_fs</t>
   </si>
 </sst>
 </file>
@@ -220,25 +241,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -520,18 +541,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:G13"/>
+      <selection activeCell="B2" sqref="B2:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="13.5" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="8.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="13.5" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -558,10 +579,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3">
@@ -571,7 +592,7 @@
         <v>134</v>
       </c>
       <c r="E2" s="3">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F2" s="3">
         <v>25</v>
@@ -581,8 +602,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3">
@@ -602,8 +623,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3">
@@ -623,10 +644,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="3">
@@ -636,7 +657,7 @@
         <v>321</v>
       </c>
       <c r="E5" s="3">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F5" s="3">
         <v>87</v>
@@ -646,29 +667,29 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="3">
         <v>1024</v>
       </c>
       <c r="D6" s="3">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E6" s="3">
-        <v>778</v>
+        <v>583</v>
       </c>
       <c r="F6" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G6" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="3">
@@ -678,7 +699,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="3">
         <v>13</v>
@@ -688,8 +709,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="3">
@@ -709,18 +730,18 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3">
         <v>1215</v>
       </c>
       <c r="D9" s="3">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="3">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F9" s="3">
         <v>1</v>
@@ -730,8 +751,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="3">
@@ -741,7 +762,7 @@
         <v>19</v>
       </c>
       <c r="E10" s="3">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
@@ -751,8 +772,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="3">
@@ -772,8 +793,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="3">
@@ -783,7 +804,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="3">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
@@ -793,29 +814,305 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10">
+      <c r="B13" s="7"/>
+      <c r="C13" s="6">
         <f>SUM(C2:C12)</f>
         <v>5616</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="6">
         <f>SUM(D2:D12)</f>
         <v>1207</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="6">
         <f>SUM(E2:E12)</f>
-        <v>1685</v>
-      </c>
-      <c r="F13" s="10">
+        <v>1475</v>
+      </c>
+      <c r="F13" s="6">
         <f>SUM(F2:F12)</f>
-        <v>166</v>
-      </c>
-      <c r="G13" s="10">
+        <v>167</v>
+      </c>
+      <c r="G13" s="6">
         <f>SUM(G2:G12)</f>
-        <v>168</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5">
+        <v>220</v>
+      </c>
+      <c r="D17" s="5">
+        <v>134</v>
+      </c>
+      <c r="E17" s="5">
+        <v>150</v>
+      </c>
+      <c r="F17" s="5">
+        <v>25</v>
+      </c>
+      <c r="G17" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="5">
+        <v>24</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" s="5">
+        <v>3</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5">
+        <v>2027</v>
+      </c>
+      <c r="D20" s="5">
+        <v>321</v>
+      </c>
+      <c r="E20" s="5">
+        <v>502</v>
+      </c>
+      <c r="F20" s="5">
+        <v>87</v>
+      </c>
+      <c r="G20" s="5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1024</v>
+      </c>
+      <c r="D21" s="5">
+        <v>540</v>
+      </c>
+      <c r="E21" s="5">
+        <v>583</v>
+      </c>
+      <c r="F21" s="5">
+        <v>38</v>
+      </c>
+      <c r="G21" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="5">
+        <v>30</v>
+      </c>
+      <c r="D22" s="5">
+        <v>17</v>
+      </c>
+      <c r="E22" s="5">
+        <v>21</v>
+      </c>
+      <c r="F22" s="5">
+        <v>13</v>
+      </c>
+      <c r="G22" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="5">
+        <v>67</v>
+      </c>
+      <c r="D23" s="5">
+        <v>4</v>
+      </c>
+      <c r="E23" s="5">
+        <v>4</v>
+      </c>
+      <c r="F23" s="5">
+        <v>2</v>
+      </c>
+      <c r="G23" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1215</v>
+      </c>
+      <c r="D24" s="5">
+        <v>55</v>
+      </c>
+      <c r="E24" s="5">
+        <v>61</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5">
+        <v>569</v>
+      </c>
+      <c r="D25" s="5">
+        <v>19</v>
+      </c>
+      <c r="E25" s="5">
+        <v>27</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="5">
+        <v>77</v>
+      </c>
+      <c r="D26" s="5">
+        <v>76</v>
+      </c>
+      <c r="E26" s="5">
+        <v>78</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="5">
+        <v>361</v>
+      </c>
+      <c r="D27" s="5">
+        <v>38</v>
+      </c>
+      <c r="E27" s="5">
+        <v>46</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The MoxR family ATPase was added to the list of queries
</commit_message>
<xml_diff>
--- a/images/statistics_table.xlsx
+++ b/images/statistics_table.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Archaea</t>
   </si>
@@ -90,27 +90,6 @@
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>kingdom</t>
-  </si>
-  <si>
-    <t>phylum2</t>
-  </si>
-  <si>
-    <t>total_orgs</t>
-  </si>
-  <si>
-    <t>orgs_with_M</t>
-  </si>
-  <si>
-    <t>num_M_genes</t>
-  </si>
-  <si>
-    <t>orgs_with_bchlD_fs</t>
-  </si>
-  <si>
-    <t>num_bchlD_fs</t>
   </si>
 </sst>
 </file>
@@ -541,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,7 +783,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
@@ -828,7 +807,7 @@
       </c>
       <c r="E13" s="6">
         <f>SUM(E2:E12)</f>
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="F13" s="6">
         <f>SUM(F2:F12)</f>
@@ -837,282 +816,6 @@
       <c r="G13" s="6">
         <f>SUM(G2:G12)</f>
         <v>169</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="5">
-        <v>220</v>
-      </c>
-      <c r="D17" s="5">
-        <v>134</v>
-      </c>
-      <c r="E17" s="5">
-        <v>150</v>
-      </c>
-      <c r="F17" s="5">
-        <v>25</v>
-      </c>
-      <c r="G17" s="5">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="5">
-        <v>24</v>
-      </c>
-      <c r="D18" s="5">
-        <v>3</v>
-      </c>
-      <c r="E18" s="5">
-        <v>3</v>
-      </c>
-      <c r="F18" s="5">
-        <v>0</v>
-      </c>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="5">
-        <v>2</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0</v>
-      </c>
-      <c r="E19" s="5">
-        <v>0</v>
-      </c>
-      <c r="F19" s="5">
-        <v>0</v>
-      </c>
-      <c r="G19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="5">
-        <v>2027</v>
-      </c>
-      <c r="D20" s="5">
-        <v>321</v>
-      </c>
-      <c r="E20" s="5">
-        <v>502</v>
-      </c>
-      <c r="F20" s="5">
-        <v>87</v>
-      </c>
-      <c r="G20" s="5">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1024</v>
-      </c>
-      <c r="D21" s="5">
-        <v>540</v>
-      </c>
-      <c r="E21" s="5">
-        <v>583</v>
-      </c>
-      <c r="F21" s="5">
-        <v>38</v>
-      </c>
-      <c r="G21" s="5">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="5">
-        <v>30</v>
-      </c>
-      <c r="D22" s="5">
-        <v>17</v>
-      </c>
-      <c r="E22" s="5">
-        <v>21</v>
-      </c>
-      <c r="F22" s="5">
-        <v>13</v>
-      </c>
-      <c r="G22" s="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="5">
-        <v>67</v>
-      </c>
-      <c r="D23" s="5">
-        <v>4</v>
-      </c>
-      <c r="E23" s="5">
-        <v>4</v>
-      </c>
-      <c r="F23" s="5">
-        <v>2</v>
-      </c>
-      <c r="G23" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="5">
-        <v>1215</v>
-      </c>
-      <c r="D24" s="5">
-        <v>55</v>
-      </c>
-      <c r="E24" s="5">
-        <v>61</v>
-      </c>
-      <c r="F24" s="5">
-        <v>1</v>
-      </c>
-      <c r="G24" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="5">
-        <v>569</v>
-      </c>
-      <c r="D25" s="5">
-        <v>19</v>
-      </c>
-      <c r="E25" s="5">
-        <v>27</v>
-      </c>
-      <c r="F25" s="5">
-        <v>1</v>
-      </c>
-      <c r="G25" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="5">
-        <v>77</v>
-      </c>
-      <c r="D26" s="5">
-        <v>76</v>
-      </c>
-      <c r="E26" s="5">
-        <v>78</v>
-      </c>
-      <c r="F26" s="5">
-        <v>0</v>
-      </c>
-      <c r="G26" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="5">
-        <v>361</v>
-      </c>
-      <c r="D27" s="5">
-        <v>38</v>
-      </c>
-      <c r="E27" s="5">
-        <v>46</v>
-      </c>
-      <c r="F27" s="5">
-        <v>0</v>
-      </c>
-      <c r="G27" s="5">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Count chlD genes instead of medium subunit genes
</commit_message>
<xml_diff>
--- a/images/statistics_table.xlsx
+++ b/images/statistics_table.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Archaea</t>
   </si>
@@ -71,18 +71,6 @@
     <t>Total number of genomes</t>
   </si>
   <si>
-    <t>Genomes with medium subunit genes</t>
-  </si>
-  <si>
-    <t>Number of medium subunit genes</t>
-  </si>
-  <si>
-    <t>Genomes with frameshifted chlD genes</t>
-  </si>
-  <si>
-    <t>Number of frameshifted chlD genes</t>
-  </si>
-  <si>
     <t>Domain</t>
   </si>
   <si>
@@ -90,6 +78,40 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>kingdom</t>
+  </si>
+  <si>
+    <t>phylum2</t>
+  </si>
+  <si>
+    <t>total_orgs</t>
+  </si>
+  <si>
+    <t>orgs_with_bchlD</t>
+  </si>
+  <si>
+    <t>num_bchlD</t>
+  </si>
+  <si>
+    <t>orgs_with_bchlD_fs</t>
+  </si>
+  <si>
+    <t>num_bchlD_fs</t>
+  </si>
+  <si>
+    <t>Genomes with chlD genes</t>
+  </si>
+  <si>
+    <t>Number of chlD genes</t>
+  </si>
+  <si>
+    <t>Genomes with fs-chlD genes</t>
+  </si>
+  <si>
+    <t>Number of
+fs-chlD genes</t>
   </si>
 </sst>
 </file>
@@ -520,41 +542,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="13.5" style="5" customWidth="1"/>
+    <col min="3" max="6" width="13.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="5" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -636,7 +659,7 @@
         <v>321</v>
       </c>
       <c r="E5" s="3">
-        <v>502</v>
+        <v>337</v>
       </c>
       <c r="F5" s="3">
         <v>87</v>
@@ -657,7 +680,7 @@
         <v>540</v>
       </c>
       <c r="E6" s="3">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="F6" s="3">
         <v>38</v>
@@ -794,7 +817,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="6">
@@ -807,7 +830,7 @@
       </c>
       <c r="E13" s="6">
         <f>SUM(E2:E12)</f>
-        <v>1476</v>
+        <v>1300</v>
       </c>
       <c r="F13" s="6">
         <f>SUM(F2:F12)</f>
@@ -816,6 +839,282 @@
       <c r="G13" s="6">
         <f>SUM(G2:G12)</f>
         <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>220</v>
+      </c>
+      <c r="D16" s="5">
+        <v>134</v>
+      </c>
+      <c r="E16" s="5">
+        <v>150</v>
+      </c>
+      <c r="F16" s="5">
+        <v>25</v>
+      </c>
+      <c r="G16" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5">
+        <v>24</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5">
+        <v>3</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2027</v>
+      </c>
+      <c r="D19" s="5">
+        <v>321</v>
+      </c>
+      <c r="E19" s="5">
+        <v>337</v>
+      </c>
+      <c r="F19" s="5">
+        <v>87</v>
+      </c>
+      <c r="G19" s="5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1024</v>
+      </c>
+      <c r="D20" s="5">
+        <v>540</v>
+      </c>
+      <c r="E20" s="5">
+        <v>572</v>
+      </c>
+      <c r="F20" s="5">
+        <v>38</v>
+      </c>
+      <c r="G20" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="5">
+        <v>30</v>
+      </c>
+      <c r="D21" s="5">
+        <v>17</v>
+      </c>
+      <c r="E21" s="5">
+        <v>21</v>
+      </c>
+      <c r="F21" s="5">
+        <v>13</v>
+      </c>
+      <c r="G21" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="5">
+        <v>67</v>
+      </c>
+      <c r="D22" s="5">
+        <v>4</v>
+      </c>
+      <c r="E22" s="5">
+        <v>4</v>
+      </c>
+      <c r="F22" s="5">
+        <v>2</v>
+      </c>
+      <c r="G22" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1215</v>
+      </c>
+      <c r="D23" s="5">
+        <v>55</v>
+      </c>
+      <c r="E23" s="5">
+        <v>61</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="5">
+        <v>569</v>
+      </c>
+      <c r="D24" s="5">
+        <v>19</v>
+      </c>
+      <c r="E24" s="5">
+        <v>27</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="5">
+        <v>77</v>
+      </c>
+      <c r="D25" s="5">
+        <v>76</v>
+      </c>
+      <c r="E25" s="5">
+        <v>78</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="5">
+        <v>361</v>
+      </c>
+      <c r="D26" s="5">
+        <v>38</v>
+      </c>
+      <c r="E26" s="5">
+        <v>47</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>